<commit_message>
hadoop cluster conf for 2 node
</commit_message>
<xml_diff>
--- a/hammer-project/hadoop_conf/hadoop yarn configurator.xlsx
+++ b/hammer-project/hadoop_conf/hadoop yarn configurator.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauropelucchi/git/hammerdataproject/hammer-project/hadoop_conf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauropelucchi/Desktop/My_Home/Git/hammerdataproject/hammer-project/hadoop_conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>YARN</t>
   </si>
@@ -102,6 +103,9 @@
   </si>
   <si>
     <t>set this row with max avaiable ram amount for 1 reduce task</t>
+  </si>
+  <si>
+    <t>2 map + 2 reduce</t>
   </si>
 </sst>
 </file>
@@ -460,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,4 +675,222 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1536</v>
+      </c>
+      <c r="D3" s="4">
+        <f>C3*2</f>
+        <v>3072</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1536</v>
+      </c>
+      <c r="D12" s="4">
+        <f>C12</f>
+        <v>1536</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <f>C3/C12</f>
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f>D3/D12</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <f>C4/C14</f>
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f>D4/D14</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="6">
+        <f>MIN(C15,C13)</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
+        <f>MIN(D15,D13)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1536</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1536</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <f>C3/C22</f>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f>D3/D22</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <f>C4/C24</f>
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f>D4/D24</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="6">
+        <f>MIN(C25,C23)</f>
+        <v>1</v>
+      </c>
+      <c r="D26" s="6">
+        <f>MIN(D25,D23)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>